<commit_message>
Minor change to graph plotting
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audio Lab\Documents\GitHub\VersionTwo\ABStaircaseMethod\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Files\jtc519 - Jacob Cooper\Listening Tests - May '23\ABStaircaseMethod\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77338E2-1332-4486-8FEA-2CF3A9253078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303D68C8-3B6C-4F84-94A8-10A281A2253D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="2" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
     <col min="4" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>